<commit_message>
Deploy-d zoriulj code-oo shinechilev
</commit_message>
<xml_diff>
--- a/_export/summary.xlsx
+++ b/_export/summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
   <si>
     <t>site</t>
   </si>
@@ -79,10 +79,13 @@
     <t>2025-11-20</t>
   </si>
   <si>
+    <t>2025-11-24</t>
+  </si>
+  <si>
     <t>https://www.facebook.com/reel/4123467941205726</t>
   </si>
   <si>
-    <t>https://bit.ly/KB-11-11</t>
+    <t>https://www.zangia.mn/</t>
   </si>
   <si>
     <t>https://exchange.boost.mn/ad/web/fdfc95aa-90ae-4871-a1b1-0428fdd37f0e</t>
@@ -133,6 +136,9 @@
     <t>https://banner.bolor.net/pub/jump?t=b9619fe07489de6d9a73d897ec39856a</t>
   </si>
   <si>
+    <t>https://ticketing.urgoo.mn/movie/HO00001798</t>
+  </si>
+  <si>
     <t>https://content.ikon.mn/raw/2025/11/11/18439/Sport_app_ikon_banner_1360x200_2.jpg</t>
   </si>
   <si>
@@ -190,76 +196,82 @@
     <t>https://content.ikon.mn/raw/2025/11/12/18446/IKON__2___1_.jpg</t>
   </si>
   <si>
-    <t>C:\Scraper\banner_screenshots\ikon_1763635528_1_649361d9.png</t>
+    <t>https://content.ikon.mn/raw/2025/11/12/18443/Banner560x400.jpg</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\ikon_1763962869_1_649361d9.png</t>
   </si>
   <si>
     <t>C:\Scraper\banner_screenshots\ikon_1763635541_1_79d16520.png</t>
   </si>
   <si>
-    <t>C:\Scraper\banner_screenshots\ikon_1763635554_1_6d7e63d1.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\ikon_1763635561_2_26cd4c0c.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\lemonpress_1763629564_0_f3725195.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\lemonpress_1763629564_1_11f86d75.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\lemonpress_1763629564_2_a8f35df3.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\lemonpress_1763629565_3_f6335426.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\lemonpress_1763629565_4_50b5be95.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\news_1763635513_5_167ecfe9.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\news_1763635515_20_767f822f.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\news_1763635517_61_d480f558.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\news_1763635529_62_09be910d.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\news_1763635537_7_5d66d2ef.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\bolortoli_1763629595_0_988754e7.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\bolortoli_1763629603_0_dc08ebf8.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\bolortoli_1763629587_0_2f23e314.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\gogo_1763635515_26_ef6fd160.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\gogo_1763635517_34_020787f6.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\gogo_1763635522_135_e2d53d38.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\bolortoli_1763635590_0_fa84a932.png</t>
-  </si>
-  <si>
-    <t>C:\Scraper\banner_screenshots\bolortoli_1763635598_0_4488d123.png</t>
+    <t>C:\Scraper\banner_screenshots\ikon_1763962886_2_6d7e63d1.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\ikon_1763954642_2_26cd4c0c.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\lemonpress_1763962920_0_f3725195.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\lemonpress_1763962920_1_11f86d75.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\lemonpress_1763962920_2_a8f35df3.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\lemonpress_1763962921_3_f6335426.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\lemonpress_1763962921_4_50b5be95.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\news_1763962859_5_167ecfe9.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\news_1763962863_20_767f822f.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\news_1763962865_62_d480f558.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\news_1763962892_63_09be910d.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\news_1763962910_7_5d66d2ef.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\bolortoli_1763962956_0_988754e7.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\bolortoli_1763962964_0_dc08ebf8.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\bolortoli_1763962973_0_2f23e314.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\gogo_1763962857_26_ef6fd160.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\gogo_1763962859_35_020787f6.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\gogo_1763962867_141_e2d53d38.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\bolortoli_1763954739_0_fa84a932.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\bolortoli_1763954768_0_4488d123.png</t>
   </si>
   <si>
     <t>C:\Scraper\banner_screenshots\bolortoli_1763635606_0_cc6f2fd0.png</t>
   </si>
   <si>
-    <t>C:\Scraper\banner_screenshots\ikon_1763629540_1_77abb1bd.png</t>
+    <t>C:\Scraper\banner_screenshots\ikon_1763962881_1_77abb1bd.png</t>
+  </si>
+  <si>
+    <t>C:\Scraper\banner_screenshots\ikon_1763962893_1_8943e5e1.png</t>
   </si>
   <si>
     <t>from_ad_page:https://ikon.mn/ad/IKONMN_A1?1763616287</t>
@@ -281,6 +293,9 @@
   </si>
   <si>
     <t>from_ad_page:https://ikon.mn/ad/IKONMN_B1?1763619886</t>
+  </si>
+  <si>
+    <t>from_ad_page:https://ikon.mn/ad/IKONMN_B2?1763954033</t>
   </si>
 </sst>
 </file>
@@ -661,7 +676,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -743,22 +758,22 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -767,10 +782,10 @@
         <v>45981.23287239583</v>
       </c>
       <c r="N2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="O2" s="3">
-        <v>45981.4529702662</v>
+        <v>45985.24167697917</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -796,10 +811,10 @@
         <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -808,7 +823,7 @@
         <v>45981.23287303241</v>
       </c>
       <c r="N3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="O3" s="3">
         <v>45981.45297028935</v>
@@ -828,22 +843,22 @@
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -852,10 +867,10 @@
         <v>45981.23287306713</v>
       </c>
       <c r="N4" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O4" s="3">
-        <v>45981.45297030092</v>
+        <v>45985.24167704861</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -872,22 +887,22 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -896,10 +911,10 @@
         <v>45981.2328730787</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="O5" s="3">
-        <v>45981.4529703125</v>
+        <v>45985.14627177083</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -916,22 +931,22 @@
         <v>20</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -940,10 +955,10 @@
         <v>45981.23287309028</v>
       </c>
       <c r="N6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O6" s="3">
-        <v>45981.38351530093</v>
+        <v>45985.24167706018</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -960,22 +975,22 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -984,10 +999,10 @@
         <v>45981.23287309028</v>
       </c>
       <c r="N7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O7" s="3">
-        <v>45981.3835153125</v>
+        <v>45985.24167708333</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1004,22 +1019,22 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1028,10 +1043,10 @@
         <v>45981.23287310185</v>
       </c>
       <c r="N8" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O8" s="3">
-        <v>45981.38351532407</v>
+        <v>45985.24167710648</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1048,22 +1063,22 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1072,10 +1087,10 @@
         <v>45981.23287310185</v>
       </c>
       <c r="N9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O9" s="3">
-        <v>45981.38351534722</v>
+        <v>45985.24167711806</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1092,22 +1107,22 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1116,10 +1131,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N10" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O10" s="3">
-        <v>45981.38351537037</v>
+        <v>45985.24167712963</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1136,22 +1151,22 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1160,10 +1175,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O11" s="3">
-        <v>45981.45297032408</v>
+        <v>45985.2416771412</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1180,22 +1195,22 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="J12" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1204,10 +1219,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N12" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O12" s="3">
-        <v>45981.45297032408</v>
+        <v>45985.24167716435</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1224,22 +1239,22 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1248,10 +1263,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N13" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O13" s="3">
-        <v>45981.45297032408</v>
+        <v>45985.24167717592</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1268,22 +1283,22 @@
         <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1292,10 +1307,10 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N14" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O14" s="3">
-        <v>45981.45297033565</v>
+        <v>45985.24167722222</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1312,22 +1327,22 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G15">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J15" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1336,10 +1351,10 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N15" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="O15" s="3">
-        <v>45981.45297033565</v>
+        <v>45985.2416772338</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1356,22 +1371,22 @@
         <v>20</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J16" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1380,10 +1395,10 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N16" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O16" s="3">
-        <v>45981.38351550926</v>
+        <v>45985.24167725694</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1400,22 +1415,22 @@
         <v>20</v>
       </c>
       <c r="E17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J17" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1424,10 +1439,10 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N17" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O17" s="3">
-        <v>45981.38351552084</v>
+        <v>45985.24167728009</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1444,22 +1459,22 @@
         <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J18" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1468,10 +1483,10 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N18" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O18" s="3">
-        <v>45981.38351546296</v>
+        <v>45985.24167729167</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1488,22 +1503,22 @@
         <v>20</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J19" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1512,10 +1527,10 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N19" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O19" s="3">
-        <v>45981.45297038194</v>
+        <v>45985.24167730324</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1532,22 +1547,22 @@
         <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G20">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="J20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1556,10 +1571,10 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N20" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O20" s="3">
-        <v>45981.45297040509</v>
+        <v>45985.24167732639</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1576,22 +1591,22 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J21" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1600,10 +1615,10 @@
         <v>45981.23287315972</v>
       </c>
       <c r="N21" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="O21" s="3">
-        <v>45981.45297041666</v>
+        <v>45985.24167738426</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1620,22 +1635,22 @@
         <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J22" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1644,10 +1659,10 @@
         <v>45981.24228215278</v>
       </c>
       <c r="N22" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O22" s="3">
-        <v>45981.4529703588</v>
+        <v>45985.14627189815</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1664,22 +1679,22 @@
         <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J23" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1688,10 +1703,10 @@
         <v>45981.24228216435</v>
       </c>
       <c r="N23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O23" s="3">
-        <v>45981.4529703588</v>
+        <v>45985.14627192129</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1717,13 +1732,13 @@
         <v>3</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J24" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1732,7 +1747,7 @@
         <v>45981.24228217592</v>
       </c>
       <c r="N24" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="O24" s="3">
         <v>45981.45297038194</v>
@@ -1752,22 +1767,22 @@
         <v>20</v>
       </c>
       <c r="E25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J25" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1776,10 +1791,54 @@
         <v>45981.27268214121</v>
       </c>
       <c r="N25" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O25" s="3">
-        <v>45981.38351528935</v>
+        <v>45985.24167701389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26">
+        <v>1280</v>
+      </c>
+      <c r="C26">
+        <v>720</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J26" t="s">
+        <v>85</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="M26" s="3">
+        <v>45985.14627177083</v>
+      </c>
+      <c r="N26" t="s">
+        <v>93</v>
+      </c>
+      <c r="O26" s="3">
+        <v>45985.24167706018</v>
       </c>
     </row>
   </sheetData>
@@ -1831,6 +1890,8 @@
     <hyperlink ref="I24" r:id="rId45"/>
     <hyperlink ref="H25" r:id="rId46"/>
     <hyperlink ref="I25" r:id="rId47"/>
+    <hyperlink ref="H26" r:id="rId48"/>
+    <hyperlink ref="I26" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
yu c gsn ajiljiga
</commit_message>
<xml_diff>
--- a/_export/summary.xlsx
+++ b/_export/summary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="196">
   <si>
     <t>site</t>
   </si>
@@ -238,6 +238,9 @@
     <t>https://banner.bolor.net/pub/jump?t=379749266bd372848d7ab4bc882c9c77</t>
   </si>
   <si>
+    <t>https://applepay.m-bank.mn/</t>
+  </si>
+  <si>
     <t>https://www.khanbank.com/personal/news/intelligence/7854/</t>
   </si>
   <si>
@@ -397,22 +400,22 @@
     <t>C:\Scraper\banner_screenshots\ikon_1764152521_1_26cd4c0c.png</t>
   </si>
   <si>
-    <t>banner_screenshots/lemonpress_1766383421_0_f3725195.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/lemonpress_1766383422_1_11f86d75.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/lemonpress_1766383422_2_a8f35df3.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/lemonpress_1766383422_3_f6335426.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/lemonpress_1766383422_4_50b5be95.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/news_1766383190_6_167ecfe9.png</t>
+    <t>banner_screenshots/lemonpress_1766396894_0_f3725195.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/lemonpress_1766396894_1_11f86d75.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/lemonpress_1766396894_2_a8f35df3.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/lemonpress_1766396895_3_f6335426.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/lemonpress_1766396895_4_50b5be95.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/news_1766396657_6_167ecfe9.png</t>
   </si>
   <si>
     <t>C:\Scraper\banner_screenshots\news_1764152503_20_767f822f.png</t>
@@ -427,7 +430,7 @@
     <t>C:\Scraper\banner_screenshots\news_1764152525_7_5d66d2ef.png</t>
   </si>
   <si>
-    <t>banner_screenshots/bolortoli_1766383463_0_988754e7.png</t>
+    <t>banner_screenshots/bolortoli_1766396948_0_988754e7.png</t>
   </si>
   <si>
     <t>C:\Scraper\banner_screenshots\bolortoli_1763962964_0_dc08ebf8.png</t>
@@ -439,10 +442,10 @@
     <t>C:\Scraper\banner_screenshots\gogo_1764152501_26_ef6fd160.png</t>
   </si>
   <si>
-    <t>banner_screenshots/gogo_1766383098_35_020787f6.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/gogo_1766383102_141_e2d53d38.png</t>
+    <t>banner_screenshots/gogo_1766396582_36_020787f6.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/gogo_1766396587_142_e2d53d38.png</t>
   </si>
   <si>
     <t>C:\Scraper\banner_screenshots\bolortoli_1763954739_0_fa84a932.png</t>
@@ -484,43 +487,43 @@
     <t>banner_screenshots/ikon_1765791769_2_2b66b92a.png</t>
   </si>
   <si>
-    <t>banner_screenshots/news_1766383176_5_1c5efbf5.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/news_1766383179_22_b35122f0.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/news_1766383180_64_63744233.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/news_1766383181_69_ccf95ae7.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/news_1766383192_23_5099a424.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/gogo_1765791721_26_e5a1225e.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/caak_1766383422_0_e8a3ee95.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/caak_1766376360_1_1dc68725.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/bolortoli_1766383497_0_bd18a737.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/bolortoli_1766383455_0_5a32e6f1.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/bolortoli_1766383472_0_e48d3301.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/ikon_1766383126_2_07def81d.png</t>
-  </si>
-  <si>
-    <t>banner_screenshots/ikon_1766378932_1_b76fdb5d.png</t>
+    <t>banner_screenshots/news_1766396645_5_1c5efbf5.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/news_1766396647_22_b35122f0.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/news_1766396648_64_63744233.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/news_1766396648_69_ccf95ae7.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/news_1766396659_23_5099a424.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/gogo_1766396580_26_e5a1225e.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/caak_1766396878_0_e8a3ee95.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/caak_1766396881_1_1dc68725.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/bolortoli_1766396923_0_bd18a737.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/bolortoli_1766396940_0_5a32e6f1.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/bolortoli_1766396973_0_e48d3301.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/ikon_1766396598_1_07def81d.png</t>
+  </si>
+  <si>
+    <t>banner_screenshots/ikon_1766396619_1_b76fdb5d.png</t>
   </si>
   <si>
     <t>banner_screenshots/ikon_1766383148_2_f6fa2762.png</t>
@@ -532,13 +535,13 @@
     <t>banner_screenshots/caak_1766383425_1_56acdb22.png</t>
   </si>
   <si>
-    <t>banner_screenshots/bolortoli_1766383446_0_f334782e.png</t>
+    <t>banner_screenshots/bolortoli_1766396932_0_f334782e.png</t>
   </si>
   <si>
     <t>banner_screenshots/ikon_1766377899_2_1225693d.png</t>
   </si>
   <si>
-    <t>banner_screenshots/ikon_1766383137_1_7f1ee0a6.png</t>
+    <t>banner_screenshots/ikon_1766396630_2_7f1ee0a6.png</t>
   </si>
   <si>
     <t>3</t>
@@ -1077,10 +1080,10 @@
         <v>39</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1089,7 +1092,7 @@
         <v>45981.23287239583</v>
       </c>
       <c r="N2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="O2" s="3">
         <v>45985.24167697917</v>
@@ -1121,10 +1124,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1133,7 +1136,7 @@
         <v>45981.23287303241</v>
       </c>
       <c r="N3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="O3" s="3">
         <v>45981.45297028935</v>
@@ -1168,10 +1171,10 @@
         <v>40</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1180,7 +1183,7 @@
         <v>45981.23287306713</v>
       </c>
       <c r="N4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O4" s="3">
         <v>45985.24167704861</v>
@@ -1215,10 +1218,10 @@
         <v>41</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -1227,7 +1230,7 @@
         <v>45981.2328730787</v>
       </c>
       <c r="N5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="O5" s="3">
         <v>45987.43331303241</v>
@@ -1265,7 +1268,7 @@
         <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -1274,10 +1277,10 @@
         <v>45981.23287309028</v>
       </c>
       <c r="N6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O6" s="3">
-        <v>46013.25388103009</v>
+        <v>46013.40986271991</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1309,7 +1312,7 @@
         <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1318,10 +1321,10 @@
         <v>45981.23287309028</v>
       </c>
       <c r="N7" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O7" s="3">
-        <v>46013.25388106482</v>
+        <v>46013.40986274306</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1353,7 +1356,7 @@
         <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1362,10 +1365,10 @@
         <v>45981.23287310185</v>
       </c>
       <c r="N8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O8" s="3">
-        <v>46013.25388107639</v>
+        <v>46013.40986277778</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1397,7 +1400,7 @@
         <v>45</v>
       </c>
       <c r="J9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1406,10 +1409,10 @@
         <v>45981.23287310185</v>
       </c>
       <c r="N9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O9" s="3">
-        <v>46013.25388109954</v>
+        <v>46013.4098628125</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1441,7 +1444,7 @@
         <v>46</v>
       </c>
       <c r="J10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1450,10 +1453,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O10" s="3">
-        <v>46013.25388111111</v>
+        <v>46013.40986282408</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1482,10 +1485,10 @@
         <v>47</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -1494,10 +1497,10 @@
         <v>45981.232873125</v>
       </c>
       <c r="N11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O11" s="3">
-        <v>46013.25388091435</v>
+        <v>46013.40986262731</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1526,10 +1529,10 @@
         <v>48</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -1538,7 +1541,7 @@
         <v>45981.232873125</v>
       </c>
       <c r="N12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O12" s="3">
         <v>45987.43331315972</v>
@@ -1573,10 +1576,10 @@
         <v>49</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J13" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1585,7 +1588,7 @@
         <v>45981.232873125</v>
       </c>
       <c r="N13" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O13" s="3">
         <v>45987.4333131713</v>
@@ -1620,10 +1623,10 @@
         <v>47</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1632,7 +1635,7 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O14" s="3">
         <v>45987.43331319444</v>
@@ -1667,10 +1670,10 @@
         <v>50</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1679,7 +1682,7 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N15" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O15" s="3">
         <v>45987.43331320602</v>
@@ -1714,10 +1717,10 @@
         <v>51</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1726,10 +1729,10 @@
         <v>45981.23287313657</v>
       </c>
       <c r="N16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O16" s="3">
-        <v>46013.25388119213</v>
+        <v>46013.40986292824</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1758,10 +1761,10 @@
         <v>52</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="K17">
         <v>0</v>
@@ -1770,7 +1773,7 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O17" s="3">
         <v>45985.24167728009</v>
@@ -1805,10 +1808,10 @@
         <v>53</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="J18" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1817,7 +1820,7 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N18" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O18" s="3">
         <v>45987.43331333333</v>
@@ -1852,10 +1855,10 @@
         <v>54</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J19" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1864,7 +1867,7 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O19" s="3">
         <v>45987.43331335648</v>
@@ -1899,10 +1902,10 @@
         <v>54</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J20" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1911,10 +1914,10 @@
         <v>45981.23287314815</v>
       </c>
       <c r="N20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O20" s="3">
-        <v>46013.25388097222</v>
+        <v>46013.40986268518</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1943,10 +1946,10 @@
         <v>54</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J21" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1955,10 +1958,10 @@
         <v>45981.23287315972</v>
       </c>
       <c r="N21" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="O21" s="3">
-        <v>46013.25388098379</v>
+        <v>46013.40986270834</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1987,10 +1990,10 @@
         <v>55</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J22" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1999,7 +2002,7 @@
         <v>45981.24228215278</v>
       </c>
       <c r="N22" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O22" s="3">
         <v>45985.14627189815</v>
@@ -2034,10 +2037,10 @@
         <v>56</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J23" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -2046,7 +2049,7 @@
         <v>45981.24228216435</v>
       </c>
       <c r="N23" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O23" s="3">
         <v>45987.43331334491</v>
@@ -2081,10 +2084,10 @@
         <v>57</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J24" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -2093,7 +2096,7 @@
         <v>45981.24228217592</v>
       </c>
       <c r="N24" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O24" s="3">
         <v>45987.43331333333</v>
@@ -2128,10 +2131,10 @@
         <v>41</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="J25" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -2140,7 +2143,7 @@
         <v>45981.27268214121</v>
       </c>
       <c r="N25" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="O25" s="3">
         <v>45987.43331310185</v>
@@ -2175,10 +2178,10 @@
         <v>58</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J26" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -2187,7 +2190,7 @@
         <v>45985.14627177083</v>
       </c>
       <c r="N26" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="O26" s="3">
         <v>45985.24167706018</v>
@@ -2222,10 +2225,10 @@
         <v>59</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J27" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2234,7 +2237,7 @@
         <v>45987.43331267361</v>
       </c>
       <c r="N27" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="O27" s="3">
         <v>45987.43331267361</v>
@@ -2269,22 +2272,22 @@
         <v>60</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="J28" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L28" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M28" s="3">
         <v>45987.43331329861</v>
       </c>
       <c r="N28" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O28" s="3">
         <v>45987.43331329861</v>
@@ -2319,22 +2322,22 @@
         <v>61</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="J29" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="K29" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M29" s="3">
         <v>45987.43331329861</v>
       </c>
       <c r="N29" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O29" s="3">
         <v>45987.43331329861</v>
@@ -2369,22 +2372,22 @@
         <v>62</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M30" s="3">
         <v>45987.43331331018</v>
       </c>
       <c r="N30" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O30" s="3">
         <v>45987.43331331018</v>
@@ -2419,22 +2422,22 @@
         <v>63</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="L31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="M31" s="3">
         <v>45987.43331332176</v>
       </c>
       <c r="N31" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="O31" s="3">
         <v>45987.43331332176</v>
@@ -2469,10 +2472,10 @@
         <v>64</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -2481,7 +2484,7 @@
         <v>46006.40792114583</v>
       </c>
       <c r="N32" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="O32" s="3">
         <v>46013.2538807176</v>
@@ -2513,10 +2516,10 @@
         <v>65</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="J33" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -2525,7 +2528,7 @@
         <v>46006.4079212037</v>
       </c>
       <c r="N33" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="O33" s="3">
         <v>46010.31155962963</v>
@@ -2557,10 +2560,10 @@
         <v>66</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="J34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="K34">
         <v>0</v>
@@ -2569,7 +2572,7 @@
         <v>46006.40792121528</v>
       </c>
       <c r="N34" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="O34" s="3">
         <v>46006.40792121528</v>
@@ -2601,10 +2604,10 @@
         <v>50</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J35" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -2613,10 +2616,10 @@
         <v>46006.40792121528</v>
       </c>
       <c r="N35" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O35" s="3">
-        <v>46013.25388081018</v>
+        <v>46013.40986256945</v>
       </c>
     </row>
     <row r="36" spans="1:15">
@@ -2645,10 +2648,10 @@
         <v>67</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J36" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K36">
         <v>0</v>
@@ -2657,10 +2660,10 @@
         <v>46006.40792122686</v>
       </c>
       <c r="N36" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O36" s="3">
-        <v>46013.25388084491</v>
+        <v>46013.40986258102</v>
       </c>
     </row>
     <row r="37" spans="1:15">
@@ -2689,10 +2692,10 @@
         <v>68</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -2701,10 +2704,10 @@
         <v>46006.40792125</v>
       </c>
       <c r="N37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O37" s="3">
-        <v>46013.25388089121</v>
+        <v>46013.40986259259</v>
       </c>
     </row>
     <row r="38" spans="1:15">
@@ -2733,10 +2736,10 @@
         <v>69</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="J38" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="K38">
         <v>0</v>
@@ -2745,10 +2748,10 @@
         <v>46006.40792126158</v>
       </c>
       <c r="N38" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O38" s="3">
-        <v>46013.25388090278</v>
+        <v>46013.40986261574</v>
       </c>
     </row>
     <row r="39" spans="1:15">
@@ -2777,10 +2780,10 @@
         <v>65</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J39" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K39">
         <v>0</v>
@@ -2789,10 +2792,10 @@
         <v>46006.40792127314</v>
       </c>
       <c r="N39" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="O39" s="3">
-        <v>46013.2538809375</v>
+        <v>46013.40986265046</v>
       </c>
     </row>
     <row r="40" spans="1:15">
@@ -2812,19 +2815,19 @@
         <v>36</v>
       </c>
       <c r="F40" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>54</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J40" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K40">
         <v>0</v>
@@ -2833,10 +2836,10 @@
         <v>46006.40792127314</v>
       </c>
       <c r="N40" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O40" s="3">
-        <v>46006.40792127314</v>
+        <v>46013.40986266204</v>
       </c>
     </row>
     <row r="41" spans="1:15">
@@ -2865,25 +2868,25 @@
         <v>70</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J41" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="K41" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L41" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M41" s="3">
         <v>46006.40792130787</v>
       </c>
       <c r="N41" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O41" s="3">
-        <v>46013.25388112268</v>
+        <v>46013.40986283565</v>
       </c>
     </row>
     <row r="42" spans="1:15">
@@ -2912,25 +2915,25 @@
         <v>65</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J42" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K42" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L42" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M42" s="3">
         <v>46006.40792130787</v>
       </c>
       <c r="N42" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O42" s="3">
-        <v>46013.17186355324</v>
+        <v>46013.4098628588</v>
       </c>
     </row>
     <row r="43" spans="1:15">
@@ -2959,10 +2962,10 @@
         <v>71</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J43" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="K43">
         <v>0</v>
@@ -2971,10 +2974,10 @@
         <v>46006.40792131944</v>
       </c>
       <c r="N43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O43" s="3">
-        <v>46013.25388122685</v>
+        <v>46013.40986287037</v>
       </c>
     </row>
     <row r="44" spans="1:15">
@@ -3003,10 +3006,10 @@
         <v>72</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J44" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="K44">
         <v>0</v>
@@ -3015,10 +3018,10 @@
         <v>46006.40792131944</v>
       </c>
       <c r="N44" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O44" s="3">
-        <v>46013.25388118056</v>
+        <v>46013.40986290509</v>
       </c>
     </row>
     <row r="45" spans="1:15">
@@ -3047,10 +3050,10 @@
         <v>73</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J45" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K45">
         <v>0</v>
@@ -3059,10 +3062,10 @@
         <v>46006.40792131944</v>
       </c>
       <c r="N45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O45" s="3">
-        <v>46013.25388121528</v>
+        <v>46013.40986296297</v>
       </c>
     </row>
     <row r="46" spans="1:15">
@@ -3070,7 +3073,7 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C46">
         <v>1280</v>
@@ -3088,13 +3091,13 @@
         <v>2</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -3103,10 +3106,10 @@
         <v>46010.29087371528</v>
       </c>
       <c r="N46" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="O46" s="3">
-        <v>46013.25388074074</v>
+        <v>46013.40986239583</v>
       </c>
     </row>
     <row r="47" spans="1:15">
@@ -3135,10 +3138,10 @@
         <v>66</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J47" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="K47">
         <v>0</v>
@@ -3147,10 +3150,10 @@
         <v>46010.29087402778</v>
       </c>
       <c r="N47" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O47" s="3">
-        <v>46013.20368797454</v>
+        <v>46013.4098625</v>
       </c>
     </row>
     <row r="48" spans="1:15">
@@ -3179,10 +3182,10 @@
         <v>66</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J48" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="K48">
         <v>0</v>
@@ -3191,7 +3194,7 @@
         <v>46010.29087403935</v>
       </c>
       <c r="N48" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="O48" s="3">
         <v>46013.25388077546</v>
@@ -3223,10 +3226,10 @@
         <v>54</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="J49" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="K49">
         <v>0</v>
@@ -3235,7 +3238,7 @@
         <v>46010.2908740625</v>
       </c>
       <c r="N49" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O49" s="3">
         <v>46013.25388094907</v>
@@ -3264,25 +3267,25 @@
         <v>2</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J50" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K50" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="L50" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M50" s="3">
         <v>46010.29087409722</v>
       </c>
       <c r="N50" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O50" s="3">
         <v>46013.25388113426</v>
@@ -3311,13 +3314,13 @@
         <v>2</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J51" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K51">
         <v>0</v>
@@ -3326,10 +3329,10 @@
         <v>46010.2908741088</v>
       </c>
       <c r="N51" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O51" s="3">
-        <v>46013.2538811574</v>
+        <v>46013.40986288194</v>
       </c>
     </row>
     <row r="52" spans="1:15">
@@ -3358,10 +3361,10 @@
         <v>66</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="J52" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="K52">
         <v>0</v>
@@ -3370,7 +3373,7 @@
         <v>46013.17186259259</v>
       </c>
       <c r="N52" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="O52" s="3">
         <v>46013.19294402777</v>
@@ -3402,10 +3405,10 @@
         <v>66</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J53" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="K53">
         <v>0</v>
@@ -3414,10 +3417,10 @@
         <v>46013.20368798611</v>
       </c>
       <c r="N53" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="O53" s="3">
-        <v>46013.25388076389</v>
+        <v>46013.40986253473</v>
       </c>
     </row>
   </sheetData>

</xml_diff>